<commit_message>
Get and display final grade, populate parts of grade column
</commit_message>
<xml_diff>
--- a/grades-example.xlsx
+++ b/grades-example.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="COMP3804" sheetId="1" state="visible" r:id="rId1"/>
@@ -372,9 +372,9 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -384,12 +384,12 @@
     <col customWidth="1" max="4" min="4" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -403,7 +403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -416,8 +416,11 @@
       <c r="D3" t="n">
         <v>76</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="n">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -430,8 +433,11 @@
       <c r="D4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="n">
+        <v>9.545454545454547</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -444,8 +450,11 @@
       <c r="D5" s="2" t="n">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -458,8 +467,11 @@
       <c r="D6" t="n">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="n">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -472,8 +484,11 @@
       <c r="D7" t="n">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="n">
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -486,8 +501,11 @@
       <c r="D8" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="n">
+        <v>8.289473684210527</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -499,6 +517,9 @@
       </c>
       <c r="D9" s="2" t="n">
         <v>0.8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -512,10 +533,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
@@ -524,12 +545,12 @@
     <col customWidth="1" max="4" min="4" width="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -543,7 +564,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -554,10 +575,13 @@
         <v>10</v>
       </c>
       <c r="D3" t="n">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>86.56</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8.656000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -567,11 +591,14 @@
       <c r="C4" t="n">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" t="n">
+        <v>100</v>
+      </c>
+      <c r="E4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -582,10 +609,13 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>0.84</v>
+      </c>
+      <c r="E5" t="n">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -598,8 +628,11 @@
       <c r="D6" t="n">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="n">
+        <v>8.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -609,11 +642,11 @@
       <c r="C7" t="n">
         <v>15</v>
       </c>
-      <c r="D7" t="n">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -623,11 +656,14 @@
       <c r="C8" t="n">
         <v>15</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -640,6 +676,12 @@
       <c r="D9" s="2" t="n">
         <v>0.8</v>
       </c>
+      <c r="E9" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="D10" s="2" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>